<commit_message>
Versions minutes from 31/03/2022
- Includes additional suggestion for target journal in the corresponding excel file
</commit_message>
<xml_diff>
--- a/dat/target_journals_suggestions.xlsx
+++ b/dat/target_journals_suggestions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="13020"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Target journal proposals" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
   <si>
     <t>Journal</t>
   </si>
@@ -243,6 +243,15 @@
   </si>
   <si>
     <t>https://academic.oup.com/aje/pages/Instructions_To_Authors</t>
+  </si>
+  <si>
+    <t>Open Research Europe</t>
+  </si>
+  <si>
+    <t>https://open-research-europe.ec.europa.eu/</t>
+  </si>
+  <si>
+    <t>Compliance with EU's Open Science policy</t>
   </si>
 </sst>
 </file>
@@ -588,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,6 +997,20 @@
         <v>58</v>
       </c>
     </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>75</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L3" r:id="rId1" location="about"/>
@@ -1008,13 +1031,20 @@
     <hyperlink ref="M10" r:id="rId16"/>
     <hyperlink ref="L11" r:id="rId17"/>
     <hyperlink ref="M11" r:id="rId18"/>
+    <hyperlink ref="L12" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId20"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006CD73A168BFB4848B1C73DF123199CA9" ma:contentTypeVersion="14" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fa5ef392447f90e4bc0e73a3715a2fa0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="09b9240e-754e-4b5b-97de-12bdb4d34faf" xmlns:ns4="21dd57bc-c1f1-4490-b4fd-8caec430d023" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dc33e969e380d2ffa83f182d98a95ed3" ns3:_="" ns4:_="">
     <xsd:import namespace="09b9240e-754e-4b5b-97de-12bdb4d34faf"/>
@@ -1243,12 +1273,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1259,6 +1283,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63DFB9CC-7A5C-42C7-AD7D-F3F62CC311FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="09b9240e-754e-4b5b-97de-12bdb4d34faf"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="21dd57bc-c1f1-4490-b4fd-8caec430d023"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FA41E8B-36CD-419D-8FDC-D6D8A52CC194}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1277,23 +1318,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63DFB9CC-7A5C-42C7-AD7D-F3F62CC311FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="09b9240e-754e-4b5b-97de-12bdb4d34faf"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="21dd57bc-c1f1-4490-b4fd-8caec430d023"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2572EA69-DE99-45F7-9F3A-B28D003C964E}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Target journals information updated
</commit_message>
<xml_diff>
--- a/dat/target_journals_suggestions.xlsx
+++ b/dat/target_journals_suggestions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="13020"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Target journal proposals" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="90">
   <si>
     <t>Journal</t>
   </si>
@@ -252,6 +252,48 @@
   </si>
   <si>
     <t>Compliance with EU's Open Science policy</t>
+  </si>
+  <si>
+    <t>Epidemiology</t>
+  </si>
+  <si>
+    <t>Suggested by mail (2022/05/12) after rejection by IJE</t>
+  </si>
+  <si>
+    <t>18/176</t>
+  </si>
+  <si>
+    <t>https://journals.lww.com/epidem/Pages/aboutthejournal.aspx</t>
+  </si>
+  <si>
+    <t>https://edmgr.ovid.com/epid/accounts/ifauth.htm</t>
+  </si>
+  <si>
+    <t>https://open-research-europe.ec.europa.eu/for-authors/publish-your-research/</t>
+  </si>
+  <si>
+    <t>Journal of Epidemiology and Community Health</t>
+  </si>
+  <si>
+    <t>Laura Rico</t>
+  </si>
+  <si>
+    <t>35/176</t>
+  </si>
+  <si>
+    <t>https://jech.bmj.com/pages/about/</t>
+  </si>
+  <si>
+    <t>https://jech.bmj.com/pages/authors/</t>
+  </si>
+  <si>
+    <t>1500-4000</t>
+  </si>
+  <si>
+    <t>Words</t>
+  </si>
+  <si>
+    <t>20 / 5</t>
   </si>
 </sst>
 </file>
@@ -304,7 +346,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -314,6 +356,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -597,30 +642,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" style="6" customWidth="1"/>
     <col min="3" max="3" width="19.140625" style="6" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" style="6" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" style="6" customWidth="1"/>
     <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="48.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="123" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="98.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -660,8 +709,11 @@
       <c r="M1" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="N1" s="2" t="s">
+        <v>88</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -703,7 +755,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -732,7 +784,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -771,7 +823,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -807,7 +859,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -842,7 +894,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -881,7 +933,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -910,7 +962,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -939,7 +991,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -968,7 +1020,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -997,7 +1049,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -1009,6 +1061,76 @@
       </c>
       <c r="L12" s="1" t="s">
         <v>74</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="6">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" t="s">
+        <v>36</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" t="s">
+        <v>83</v>
+      </c>
+      <c r="G14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K14" t="s">
+        <v>36</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1032,9 +1154,16 @@
     <hyperlink ref="L11" r:id="rId17"/>
     <hyperlink ref="M11" r:id="rId18"/>
     <hyperlink ref="L12" r:id="rId19"/>
+    <hyperlink ref="L13" r:id="rId20"/>
+    <hyperlink ref="M13" r:id="rId21"/>
+    <hyperlink ref="M12" r:id="rId22"/>
+    <hyperlink ref="L14" r:id="rId23"/>
+    <hyperlink ref="M14" r:id="rId24"/>
+    <hyperlink ref="L5" r:id="rId25"/>
+    <hyperlink ref="M5" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId27"/>
 </worksheet>
 </file>
 

</xml_diff>